<commit_message>
Corrección de Errores en Principal Generación del Javadoc Update de tests
</commit_message>
<xml_diff>
--- a/JavaApplication4/tiempos de corrida.xlsx
+++ b/JavaApplication4/tiempos de corrida.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\massa\Desktop\hoja3\hoja31\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooli\OneDrive\Documents\NetBeansProjects\Hoja3CC2003\JavaApplication4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="18" documentId="6994570520220BC3114ACABC94897C093226FFDE" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{347F7326-316C-4945-AA89-428438CF0335}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{07253B4F-3590-4C8E-8203-FAF32E7F2A28}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">BUBBLE </t>
   </si>
@@ -69,6 +70,33 @@
   </si>
   <si>
     <t>GNOME SORT</t>
+  </si>
+  <si>
+    <t>Tiempo teórico</t>
+  </si>
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>Gnome</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Radix</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>nlogn</t>
+  </si>
+  <si>
+    <t>kn</t>
   </si>
 </sst>
 </file>
@@ -126,7 +154,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -158,7 +186,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-GT" baseline="0"/>
-              <a:t>tiempo de ejecución (ms) </a:t>
+              <a:t>tiempo de ejecución con lista desordenada (ms) </a:t>
             </a:r>
             <a:endParaRPr lang="es-GT"/>
           </a:p>
@@ -1354,16 +1382,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1226820</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1264920</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1392,7 +1420,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1688,27 +1716,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE86D73D-CC31-4B22-855B-787D55B35037}">
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.77734375" customWidth="1"/>
     <col min="3" max="4" width="21.88671875" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
     <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -1725,7 +1754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1745,7 +1774,7 @@
         <v>62.1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1765,7 +1794,7 @@
         <v>7.48</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1785,7 +1814,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1805,7 +1834,7 @@
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1825,7 +1854,7 @@
         <v>0.158</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -1841,8 +1870,23 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -1861,8 +1905,26 @@
       <c r="G11">
         <v>0.17699999999999999</v>
       </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1944,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1902,7 +1964,7 @@
         <v>0.36899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1922,7 +1984,7 @@
         <v>0.159</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>9</v>
       </c>

</xml_diff>